<commit_message>
feat(OceanInvader) Ajout des graphiques (Mer, missiles)
</commit_message>
<xml_diff>
--- a/doc/UX/JDT_NicolaGolaz.xlsx
+++ b/doc/UX/JDT_NicolaGolaz.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\po42oio\Documents\GitHub\OceanInvader\doc\UX\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\golaz\OneDrive\Documents\GitHub\P_OceanInvader\doc\UX\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0955333-9B24-4A17-83E6-5F95A2F6C2EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DCBE36-0E47-4F60-8288-439E97127541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{6CC57B32-2488-5244-B7A6-FB7E808234AC}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal de travail" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Auteur:</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t>ABSENT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">finalisation du haute fidéliter de l'éditeur de niveau </t>
+  </si>
+  <si>
+    <t>Réalisation du gestionnaire de niveau et ajustement de certain détails sur les autre wireframe</t>
   </si>
 </sst>
 </file>
@@ -586,6 +592,80 @@
   <dxfs count="17">
     <dxf>
       <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCCC00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -759,80 +839,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCCC00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3928,18 +3934,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}" name="Table1" displayName="Table1" ref="A6:G532" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="A6:G532" xr:uid="{F2213DF1-F6B1-174C-AC17-4E96BE96C00D}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="6">
+    <tableColumn id="1" xr3:uid="{315BA4B4-9BD9-AB4E-8D40-FABFA0BB2AEA}" name="Semaine" dataDxfId="14">
       <calculatedColumnFormula>IF(ISBLANK(B7),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B7))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{503C31E9-854D-BF42-85AC-8DFA1376C4D8}" name="Jour" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{B35A0B98-71A0-BA4F-BFAB-00A05EA1F23A}" name="h.      " dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{BE4D837D-FC99-BA48-A82F-B8C8E4CE5BF8}" name="min." dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{A2DCC539-6D2A-B04A-BF8E-6FACE6268D1F}" name="Type" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{4EA406B9-7EF7-D547-AF98-5AD11BE168E9}" name="Description" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{1735360B-2647-6D42-A0E3-3425EE302FFD}" name="Remarques/problèmes" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4135,7 +4141,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F15" sqref="F15"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4190,7 +4196,7 @@
       <c r="B3" s="82"/>
       <c r="C3" s="78" t="str">
         <f>QUOTIENT(E4,60)&amp;" heures "&amp;MOD(E4,60)&amp;" minutes"</f>
-        <v>2 heures 30 minutes</v>
+        <v>6 heures 0 minutes</v>
       </c>
       <c r="D3" s="19"/>
       <c r="E3" s="3"/>
@@ -4205,15 +4211,15 @@
       <c r="B4" s="5"/>
       <c r="C4" s="19">
         <f>SUBTOTAL(9,$C$7:$C$531)*60</f>
-        <v>60</v>
+        <v>240</v>
       </c>
       <c r="D4" s="19">
         <f>SUBTOTAL(9,$D$7:$D$531)</f>
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="E4" s="29">
         <f>SUM(C4:D4)</f>
-        <v>150</v>
+        <v>360</v>
       </c>
       <c r="F4" s="4"/>
       <c r="G4" s="6"/>
@@ -4396,15 +4402,23 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="74" t="str">
+      <c r="A13" s="74">
         <f>IF(ISBLANK(B13),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B13))</f>
-        <v/>
-      </c>
-      <c r="B13" s="40"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="42"/>
+        <v>43</v>
+      </c>
+      <c r="B13" s="40">
+        <v>45591</v>
+      </c>
+      <c r="C13" s="41">
+        <v>1</v>
+      </c>
+      <c r="D13" s="42">
+        <v>30</v>
+      </c>
       <c r="E13" s="43"/>
-      <c r="F13" s="28"/>
+      <c r="F13" s="28" t="s">
+        <v>36</v>
+      </c>
       <c r="G13" s="46"/>
       <c r="N13">
         <v>6</v>
@@ -4414,15 +4428,21 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="73" t="str">
+      <c r="A14" s="73">
         <f>IF(ISBLANK(B14),"",_xlfn.ISOWEEKNUM('Journal de travail'!$B14))</f>
-        <v/>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
+        <v>43</v>
+      </c>
+      <c r="B14" s="36">
+        <v>45591</v>
+      </c>
+      <c r="C14" s="37">
+        <v>2</v>
+      </c>
       <c r="D14" s="38"/>
       <c r="E14" s="39"/>
-      <c r="F14" s="28"/>
+      <c r="F14" s="28" t="s">
+        <v>37</v>
+      </c>
       <c r="G14" s="45"/>
       <c r="N14">
         <v>7</v>
@@ -10674,28 +10694,28 @@
     <mergeCell ref="A3:B3"/>
   </mergeCells>
   <conditionalFormatting sqref="E7:E532">
-    <cfRule type="expression" dxfId="16" priority="1">
+    <cfRule type="expression" dxfId="7" priority="1">
       <formula>$E7="Autre"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="2" stopIfTrue="1">
       <formula>$E7="Design"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="3" stopIfTrue="1">
       <formula>$E7="Présentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="4" stopIfTrue="1">
       <formula>$E7="Meeting"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>$E7="Documentation"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="6" stopIfTrue="1">
       <formula>$E7="Test"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="7" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="7" stopIfTrue="1">
       <formula>$E7="Analyse"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="9" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="9" stopIfTrue="1">
       <formula>$E7="Développement"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11012,6 +11032,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="eefa3612-053e-497a-ae76-8a76877f5e22" xsi:nil="true"/>
@@ -11020,15 +11049,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11227,6 +11247,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0453EC0E-0298-408B-815C-A1500DB4F5E9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -11235,14 +11263,6 @@
     <ds:schemaRef ds:uri="99ffe1f3-7857-457f-add0-5bdef636f38d"/>
     <ds:schemaRef ds:uri="eefa3612-053e-497a-ae76-8a76877f5e22"/>
     <ds:schemaRef ds:uri="b5cf4370-ac38-4b9e-9836-ef6f5df64f24"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{74326215-CB02-4E95-BFFB-9EC625B1BF0F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>